<commit_message>
updated dataset and json files
</commit_message>
<xml_diff>
--- a/datasets/student_record.xlsx
+++ b/datasets/student_record.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Documents\Master\Thesis\Code\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD0D1C56-176B-4765-AF5F-B72E476C5561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E5FEFA-0B9D-414A-99A8-09A879C04365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student_record" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="252">
   <si>
     <t>case</t>
   </si>
@@ -626,15 +626,6 @@
   </si>
   <si>
     <t>2019-10-21T00:34:55.684Z</t>
-  </si>
-  <si>
-    <t>2019-10-21T00:35:00.706Z</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>A21</t>
   </si>
   <si>
     <t>2019-10-21T01:09:44.017Z</t>
@@ -790,7 +781,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1625,12 +1616,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="7" max="7" width="44.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -4657,7 +4665,7 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B92" t="s">
         <v>202</v>
@@ -4698,25 +4706,25 @@
         <v>22</v>
       </c>
       <c r="D93" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E93" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F93" t="s">
+        <v>32</v>
       </c>
       <c r="G93" t="s">
-        <v>206</v>
-      </c>
-      <c r="H93" t="s">
-        <v>26</v>
-      </c>
-      <c r="I93" t="s">
-        <v>27</v>
-      </c>
-      <c r="J93" t="s">
-        <v>207</v>
-      </c>
-      <c r="O93" t="s">
-        <v>206</v>
+        <v>203</v>
+      </c>
+      <c r="L93" t="s">
+        <v>33</v>
+      </c>
+      <c r="M93" t="s">
+        <v>34</v>
+      </c>
+      <c r="N93" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.35">
@@ -4724,7 +4732,7 @@
         <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C94" t="s">
         <v>22</v>
@@ -4733,13 +4741,10 @@
         <v>30</v>
       </c>
       <c r="E94" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F94" t="s">
         <v>32</v>
-      </c>
-      <c r="G94" t="s">
-        <v>206</v>
       </c>
       <c r="L94" t="s">
         <v>33</v>
@@ -4749,6 +4754,9 @@
       </c>
       <c r="N94" t="s">
         <v>35</v>
+      </c>
+      <c r="O94" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.35">
@@ -4756,31 +4764,31 @@
         <v>46</v>
       </c>
       <c r="B95" t="s">
+        <v>207</v>
+      </c>
+      <c r="C95" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" t="s">
+        <v>23</v>
+      </c>
+      <c r="E95" t="s">
+        <v>24</v>
+      </c>
+      <c r="G95" t="s">
+        <v>208</v>
+      </c>
+      <c r="H95" t="s">
+        <v>26</v>
+      </c>
+      <c r="I95" t="s">
+        <v>27</v>
+      </c>
+      <c r="J95" t="s">
         <v>209</v>
       </c>
-      <c r="C95" t="s">
-        <v>22</v>
-      </c>
-      <c r="D95" t="s">
-        <v>30</v>
-      </c>
-      <c r="E95" t="s">
-        <v>37</v>
-      </c>
-      <c r="F95" t="s">
-        <v>32</v>
-      </c>
-      <c r="L95" t="s">
-        <v>33</v>
-      </c>
-      <c r="M95" t="s">
-        <v>34</v>
-      </c>
-      <c r="N95" t="s">
-        <v>35</v>
-      </c>
       <c r="O95" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.35">
@@ -4794,22 +4802,25 @@
         <v>22</v>
       </c>
       <c r="D96" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E96" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F96" t="s">
+        <v>32</v>
       </c>
       <c r="G96" t="s">
-        <v>211</v>
-      </c>
-      <c r="H96" t="s">
-        <v>26</v>
-      </c>
-      <c r="I96" t="s">
-        <v>27</v>
-      </c>
-      <c r="J96" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="L96" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" t="s">
+        <v>34</v>
+      </c>
+      <c r="N96" t="s">
+        <v>35</v>
       </c>
       <c r="O96" t="s">
         <v>211</v>
@@ -4820,7 +4831,7 @@
         <v>46</v>
       </c>
       <c r="B97" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C97" t="s">
         <v>22</v>
@@ -4829,13 +4840,10 @@
         <v>30</v>
       </c>
       <c r="E97" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F97" t="s">
         <v>32</v>
-      </c>
-      <c r="G97" t="s">
-        <v>211</v>
       </c>
       <c r="L97" t="s">
         <v>33</v>
@@ -4847,7 +4855,7 @@
         <v>35</v>
       </c>
       <c r="O97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
@@ -4855,31 +4863,31 @@
         <v>46</v>
       </c>
       <c r="B98" t="s">
+        <v>214</v>
+      </c>
+      <c r="C98" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
+      <c r="E98" t="s">
+        <v>24</v>
+      </c>
+      <c r="G98" s="1">
+        <v>35880</v>
+      </c>
+      <c r="H98" t="s">
+        <v>26</v>
+      </c>
+      <c r="I98" t="s">
+        <v>27</v>
+      </c>
+      <c r="J98" t="s">
         <v>215</v>
       </c>
-      <c r="C98" t="s">
-        <v>22</v>
-      </c>
-      <c r="D98" t="s">
-        <v>30</v>
-      </c>
-      <c r="E98" t="s">
-        <v>37</v>
-      </c>
-      <c r="F98" t="s">
-        <v>32</v>
-      </c>
-      <c r="L98" t="s">
-        <v>33</v>
-      </c>
-      <c r="M98" t="s">
-        <v>34</v>
-      </c>
-      <c r="N98" t="s">
-        <v>35</v>
-      </c>
-      <c r="O98" t="s">
-        <v>216</v>
+      <c r="O98" s="1">
+        <v>35880</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.35">
@@ -4887,31 +4895,34 @@
         <v>46</v>
       </c>
       <c r="B99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" t="s">
         <v>22</v>
       </c>
       <c r="D99" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E99" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F99" t="s">
+        <v>32</v>
       </c>
       <c r="G99" s="1">
         <v>35880</v>
       </c>
-      <c r="H99" t="s">
-        <v>26</v>
-      </c>
-      <c r="I99" t="s">
-        <v>27</v>
-      </c>
       <c r="J99" t="s">
-        <v>218</v>
-      </c>
-      <c r="O99" s="1">
-        <v>35880</v>
+        <v>48</v>
+      </c>
+      <c r="L99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M99" t="s">
+        <v>34</v>
+      </c>
+      <c r="N99" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.35">
@@ -4919,7 +4930,7 @@
         <v>46</v>
       </c>
       <c r="B100" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C100" t="s">
         <v>22</v>
@@ -4928,13 +4939,10 @@
         <v>30</v>
       </c>
       <c r="E100" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F100" t="s">
         <v>32</v>
-      </c>
-      <c r="G100" s="1">
-        <v>35880</v>
       </c>
       <c r="J100" t="s">
         <v>48</v>
@@ -4947,6 +4955,9 @@
       </c>
       <c r="N100" t="s">
         <v>49</v>
+      </c>
+      <c r="O100" s="1">
+        <v>35880</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.35">
@@ -4954,34 +4965,31 @@
         <v>46</v>
       </c>
       <c r="B101" t="s">
+        <v>218</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s">
+        <v>24</v>
+      </c>
+      <c r="G101" t="s">
+        <v>219</v>
+      </c>
+      <c r="H101" t="s">
+        <v>26</v>
+      </c>
+      <c r="I101" t="s">
+        <v>27</v>
+      </c>
+      <c r="J101" t="s">
         <v>220</v>
       </c>
-      <c r="C101" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" t="s">
-        <v>30</v>
-      </c>
-      <c r="E101" t="s">
-        <v>37</v>
-      </c>
-      <c r="F101" t="s">
-        <v>32</v>
-      </c>
-      <c r="J101" t="s">
-        <v>48</v>
-      </c>
-      <c r="L101" t="s">
-        <v>33</v>
-      </c>
-      <c r="M101" t="s">
-        <v>34</v>
-      </c>
-      <c r="N101" t="s">
-        <v>49</v>
-      </c>
-      <c r="O101" s="1">
-        <v>35880</v>
+      <c r="O101" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.35">
@@ -4995,25 +5003,28 @@
         <v>22</v>
       </c>
       <c r="D102" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E102" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F102" t="s">
+        <v>32</v>
       </c>
       <c r="G102" t="s">
-        <v>222</v>
-      </c>
-      <c r="H102" t="s">
-        <v>26</v>
-      </c>
-      <c r="I102" t="s">
-        <v>27</v>
+        <v>219</v>
       </c>
       <c r="J102" t="s">
-        <v>223</v>
-      </c>
-      <c r="O102" t="s">
-        <v>222</v>
+        <v>55</v>
+      </c>
+      <c r="L102" t="s">
+        <v>33</v>
+      </c>
+      <c r="M102" t="s">
+        <v>34</v>
+      </c>
+      <c r="N102" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.35">
@@ -5021,7 +5032,7 @@
         <v>46</v>
       </c>
       <c r="B103" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C103" t="s">
         <v>22</v>
@@ -5030,13 +5041,10 @@
         <v>30</v>
       </c>
       <c r="E103" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F103" t="s">
         <v>32</v>
-      </c>
-      <c r="G103" t="s">
-        <v>222</v>
       </c>
       <c r="J103" t="s">
         <v>55</v>
@@ -5049,6 +5057,9 @@
       </c>
       <c r="N103" t="s">
         <v>56</v>
+      </c>
+      <c r="O103" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.35">
@@ -5056,34 +5067,31 @@
         <v>46</v>
       </c>
       <c r="B104" t="s">
+        <v>224</v>
+      </c>
+      <c r="C104" t="s">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s">
+        <v>23</v>
+      </c>
+      <c r="E104" t="s">
+        <v>24</v>
+      </c>
+      <c r="G104" t="s">
         <v>225</v>
       </c>
-      <c r="C104" t="s">
-        <v>22</v>
-      </c>
-      <c r="D104" t="s">
-        <v>30</v>
-      </c>
-      <c r="E104" t="s">
-        <v>37</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
+      <c r="H104" t="s">
+        <v>26</v>
+      </c>
+      <c r="I104" t="s">
+        <v>27</v>
       </c>
       <c r="J104" t="s">
-        <v>55</v>
-      </c>
-      <c r="L104" t="s">
-        <v>33</v>
-      </c>
-      <c r="M104" t="s">
-        <v>34</v>
-      </c>
-      <c r="N104" t="s">
-        <v>56</v>
+        <v>226</v>
       </c>
       <c r="O104" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
@@ -5097,25 +5105,25 @@
         <v>22</v>
       </c>
       <c r="D105" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E105" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F105" t="s">
+        <v>32</v>
       </c>
       <c r="G105" t="s">
-        <v>228</v>
-      </c>
-      <c r="H105" t="s">
-        <v>26</v>
-      </c>
-      <c r="I105" t="s">
-        <v>27</v>
-      </c>
-      <c r="J105" t="s">
-        <v>229</v>
-      </c>
-      <c r="O105" t="s">
-        <v>228</v>
+        <v>225</v>
+      </c>
+      <c r="L105" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" t="s">
+        <v>34</v>
+      </c>
+      <c r="N105" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
@@ -5123,7 +5131,7 @@
         <v>46</v>
       </c>
       <c r="B106" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C106" t="s">
         <v>22</v>
@@ -5132,13 +5140,10 @@
         <v>30</v>
       </c>
       <c r="E106" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F106" t="s">
         <v>32</v>
-      </c>
-      <c r="G106" t="s">
-        <v>228</v>
       </c>
       <c r="L106" t="s">
         <v>33</v>
@@ -5148,6 +5153,9 @@
       </c>
       <c r="N106" t="s">
         <v>63</v>
+      </c>
+      <c r="O106" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
@@ -5155,31 +5163,31 @@
         <v>46</v>
       </c>
       <c r="B107" t="s">
+        <v>229</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>23</v>
+      </c>
+      <c r="E107" t="s">
+        <v>24</v>
+      </c>
+      <c r="G107" t="s">
+        <v>230</v>
+      </c>
+      <c r="H107" t="s">
+        <v>26</v>
+      </c>
+      <c r="I107" t="s">
+        <v>27</v>
+      </c>
+      <c r="J107" t="s">
         <v>231</v>
       </c>
-      <c r="C107" t="s">
-        <v>22</v>
-      </c>
-      <c r="D107" t="s">
-        <v>30</v>
-      </c>
-      <c r="E107" t="s">
-        <v>37</v>
-      </c>
-      <c r="F107" t="s">
-        <v>32</v>
-      </c>
-      <c r="L107" t="s">
-        <v>33</v>
-      </c>
-      <c r="M107" t="s">
-        <v>34</v>
-      </c>
-      <c r="N107" t="s">
-        <v>63</v>
-      </c>
       <c r="O107" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.35">
@@ -5193,25 +5201,25 @@
         <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E108" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F108" t="s">
+        <v>32</v>
       </c>
       <c r="G108" t="s">
-        <v>233</v>
-      </c>
-      <c r="H108" t="s">
-        <v>26</v>
-      </c>
-      <c r="I108" t="s">
-        <v>27</v>
-      </c>
-      <c r="J108" t="s">
-        <v>234</v>
-      </c>
-      <c r="O108" t="s">
-        <v>233</v>
+        <v>230</v>
+      </c>
+      <c r="L108" t="s">
+        <v>33</v>
+      </c>
+      <c r="M108" t="s">
+        <v>34</v>
+      </c>
+      <c r="N108" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.35">
@@ -5219,7 +5227,7 @@
         <v>46</v>
       </c>
       <c r="B109" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C109" t="s">
         <v>22</v>
@@ -5228,13 +5236,10 @@
         <v>30</v>
       </c>
       <c r="E109" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F109" t="s">
         <v>32</v>
-      </c>
-      <c r="G109" t="s">
-        <v>233</v>
       </c>
       <c r="L109" t="s">
         <v>33</v>
@@ -5244,6 +5249,9 @@
       </c>
       <c r="N109" t="s">
         <v>69</v>
+      </c>
+      <c r="O109" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
@@ -5251,31 +5259,31 @@
         <v>46</v>
       </c>
       <c r="B110" t="s">
+        <v>234</v>
+      </c>
+      <c r="C110" t="s">
+        <v>22</v>
+      </c>
+      <c r="D110" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" t="s">
+        <v>24</v>
+      </c>
+      <c r="G110" t="s">
+        <v>235</v>
+      </c>
+      <c r="H110" t="s">
+        <v>26</v>
+      </c>
+      <c r="I110" t="s">
+        <v>27</v>
+      </c>
+      <c r="J110" t="s">
         <v>236</v>
       </c>
-      <c r="C110" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" t="s">
-        <v>30</v>
-      </c>
-      <c r="E110" t="s">
-        <v>37</v>
-      </c>
-      <c r="F110" t="s">
-        <v>32</v>
-      </c>
-      <c r="L110" t="s">
-        <v>33</v>
-      </c>
-      <c r="M110" t="s">
-        <v>34</v>
-      </c>
-      <c r="N110" t="s">
-        <v>69</v>
-      </c>
       <c r="O110" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
@@ -5289,25 +5297,25 @@
         <v>22</v>
       </c>
       <c r="D111" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E111" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="F111" t="s">
+        <v>32</v>
       </c>
       <c r="G111" t="s">
-        <v>238</v>
-      </c>
-      <c r="H111" t="s">
-        <v>26</v>
-      </c>
-      <c r="I111" t="s">
-        <v>27</v>
-      </c>
-      <c r="J111" t="s">
-        <v>239</v>
-      </c>
-      <c r="O111" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+      <c r="L111" t="s">
+        <v>33</v>
+      </c>
+      <c r="M111" t="s">
+        <v>34</v>
+      </c>
+      <c r="N111" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.35">
@@ -5315,7 +5323,7 @@
         <v>46</v>
       </c>
       <c r="B112" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C112" t="s">
         <v>22</v>
@@ -5324,13 +5332,10 @@
         <v>30</v>
       </c>
       <c r="E112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F112" t="s">
         <v>32</v>
-      </c>
-      <c r="G112" t="s">
-        <v>238</v>
       </c>
       <c r="L112" t="s">
         <v>33</v>
@@ -5340,6 +5345,9 @@
       </c>
       <c r="N112" t="s">
         <v>75</v>
+      </c>
+      <c r="O112" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.35">
@@ -5347,7 +5355,7 @@
         <v>46</v>
       </c>
       <c r="B113" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C113" t="s">
         <v>22</v>
@@ -5356,11 +5364,14 @@
         <v>30</v>
       </c>
       <c r="E113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F113" t="s">
         <v>32</v>
       </c>
+      <c r="G113" t="s">
+        <v>235</v>
+      </c>
       <c r="L113" t="s">
         <v>33</v>
       </c>
@@ -5368,10 +5379,7 @@
         <v>34</v>
       </c>
       <c r="N113" t="s">
-        <v>75</v>
-      </c>
-      <c r="O113" t="s">
-        <v>242</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.35">
@@ -5379,7 +5387,7 @@
         <v>46</v>
       </c>
       <c r="B114" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C114" t="s">
         <v>22</v>
@@ -5388,13 +5396,10 @@
         <v>30</v>
       </c>
       <c r="E114" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F114" t="s">
         <v>32</v>
-      </c>
-      <c r="G114" t="s">
-        <v>238</v>
       </c>
       <c r="L114" t="s">
         <v>33</v>
@@ -5404,6 +5409,9 @@
       </c>
       <c r="N114" t="s">
         <v>79</v>
+      </c>
+      <c r="O114" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.35">
@@ -5411,7 +5419,7 @@
         <v>46</v>
       </c>
       <c r="B115" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C115" t="s">
         <v>22</v>
@@ -5420,11 +5428,14 @@
         <v>30</v>
       </c>
       <c r="E115" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F115" t="s">
         <v>32</v>
       </c>
+      <c r="G115" t="s">
+        <v>235</v>
+      </c>
       <c r="L115" t="s">
         <v>33</v>
       </c>
@@ -5432,10 +5443,7 @@
         <v>34</v>
       </c>
       <c r="N115" t="s">
-        <v>79</v>
-      </c>
-      <c r="O115" t="s">
-        <v>245</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.35">
@@ -5443,31 +5451,31 @@
         <v>46</v>
       </c>
       <c r="B116" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C116" t="s">
         <v>22</v>
       </c>
       <c r="D116" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E116" t="s">
-        <v>31</v>
-      </c>
-      <c r="F116" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G116" t="s">
-        <v>238</v>
-      </c>
-      <c r="L116" t="s">
-        <v>33</v>
-      </c>
-      <c r="M116" t="s">
-        <v>34</v>
-      </c>
-      <c r="N116" t="s">
-        <v>83</v>
+        <v>235</v>
+      </c>
+      <c r="H116" t="s">
+        <v>26</v>
+      </c>
+      <c r="I116" t="s">
+        <v>27</v>
+      </c>
+      <c r="J116" t="s">
+        <v>236</v>
+      </c>
+      <c r="O116" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.35">
@@ -5475,31 +5483,31 @@
         <v>46</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
         <v>22</v>
       </c>
       <c r="D117" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E117" t="s">
-        <v>24</v>
-      </c>
-      <c r="G117" t="s">
-        <v>238</v>
-      </c>
-      <c r="H117" t="s">
-        <v>26</v>
-      </c>
-      <c r="I117" t="s">
-        <v>27</v>
-      </c>
-      <c r="J117" t="s">
-        <v>239</v>
+        <v>37</v>
+      </c>
+      <c r="F117" t="s">
+        <v>32</v>
+      </c>
+      <c r="L117" t="s">
+        <v>33</v>
+      </c>
+      <c r="M117" t="s">
+        <v>34</v>
+      </c>
+      <c r="N117" t="s">
+        <v>83</v>
       </c>
       <c r="O117" t="s">
-        <v>238</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.35">
@@ -5507,7 +5515,7 @@
         <v>46</v>
       </c>
       <c r="B118" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C118" t="s">
         <v>22</v>
@@ -5516,11 +5524,14 @@
         <v>30</v>
       </c>
       <c r="E118" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F118" t="s">
         <v>32</v>
       </c>
+      <c r="G118" t="s">
+        <v>235</v>
+      </c>
       <c r="L118" t="s">
         <v>33</v>
       </c>
@@ -5528,10 +5539,7 @@
         <v>34</v>
       </c>
       <c r="N118" t="s">
-        <v>83</v>
-      </c>
-      <c r="O118" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.35">
@@ -5539,7 +5547,7 @@
         <v>46</v>
       </c>
       <c r="B119" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C119" t="s">
         <v>22</v>
@@ -5548,13 +5556,10 @@
         <v>30</v>
       </c>
       <c r="E119" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F119" t="s">
         <v>32</v>
-      </c>
-      <c r="G119" t="s">
-        <v>238</v>
       </c>
       <c r="L119" t="s">
         <v>33</v>
@@ -5564,6 +5569,9 @@
       </c>
       <c r="N119" t="s">
         <v>87</v>
+      </c>
+      <c r="O119">
+        <v>3067</v>
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.35">
@@ -5571,7 +5579,7 @@
         <v>46</v>
       </c>
       <c r="B120" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C120" t="s">
         <v>22</v>
@@ -5580,22 +5588,28 @@
         <v>30</v>
       </c>
       <c r="E120" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="F120" t="s">
         <v>32</v>
       </c>
+      <c r="J120" t="s">
+        <v>91</v>
+      </c>
       <c r="L120" t="s">
         <v>33</v>
       </c>
       <c r="M120" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="N120" t="s">
-        <v>87</v>
-      </c>
-      <c r="O120">
-        <v>3067</v>
+        <v>91</v>
+      </c>
+      <c r="O120" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q120" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.35">
@@ -5603,7 +5617,7 @@
         <v>46</v>
       </c>
       <c r="B121" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C121" t="s">
         <v>22</v>
@@ -5612,7 +5626,7 @@
         <v>30</v>
       </c>
       <c r="E121" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="F121" t="s">
         <v>32</v>
@@ -5641,7 +5655,7 @@
         <v>46</v>
       </c>
       <c r="B122" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
         <v>22</v>
@@ -5650,28 +5664,25 @@
         <v>30</v>
       </c>
       <c r="E122" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="F122" t="s">
         <v>32</v>
       </c>
-      <c r="J122" t="s">
-        <v>91</v>
-      </c>
       <c r="L122" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="M122" t="s">
-        <v>92</v>
-      </c>
-      <c r="N122" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="O122" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q122" t="b">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="P122" t="s">
+        <v>99</v>
+      </c>
+      <c r="U122" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.35">
@@ -5679,7 +5690,7 @@
         <v>46</v>
       </c>
       <c r="B123" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
         <v>22</v>
@@ -5688,56 +5699,21 @@
         <v>30</v>
       </c>
       <c r="E123" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F123" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="L123" t="s">
-        <v>97</v>
-      </c>
-      <c r="M123" t="s">
-        <v>98</v>
-      </c>
-      <c r="O123" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="P123" t="s">
-        <v>99</v>
+        <v>105</v>
+      </c>
+      <c r="R123" t="s">
+        <v>106</v>
       </c>
       <c r="U123" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A124">
-        <v>46</v>
-      </c>
-      <c r="B124" t="s">
-        <v>254</v>
-      </c>
-      <c r="C124" t="s">
-        <v>22</v>
-      </c>
-      <c r="D124" t="s">
-        <v>30</v>
-      </c>
-      <c r="E124" t="s">
-        <v>102</v>
-      </c>
-      <c r="F124" t="s">
-        <v>103</v>
-      </c>
-      <c r="L124" t="s">
-        <v>104</v>
-      </c>
-      <c r="P124" t="s">
-        <v>105</v>
-      </c>
-      <c r="R124" t="s">
-        <v>106</v>
-      </c>
-      <c r="U124" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>